<commit_message>
PRIMER CAMBIO REPORTES XLS
</commit_message>
<xml_diff>
--- a/reportes/controladores_fpdf/template_contabilidad_1.xlsx
+++ b/reportes/controladores_fpdf/template_contabilidad_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\TRABAJO\RESPALDO\SISTEMAHONDURAS\BACKUP\reportes\controladores_fpdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DE7D3B-D7DF-40D8-B9A5-74194A7F1DDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB1BD9C-0FB2-48BB-AF04-903C56FBD4A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>FUERZAS ARMADAS DE HONDURAS</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>SALDO</t>
   </si>
   <si>
     <t>FECHA</t>
@@ -159,7 +156,7 @@
       <name val="Lucida Sans Unicode"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,19 +184,6 @@
       </gradientFill>
     </fill>
     <fill>
-      <gradientFill degree="90">
-        <stop position="0">
-          <color theme="0"/>
-        </stop>
-        <stop position="0.5">
-          <color theme="4" tint="0.40000610370189521"/>
-        </stop>
-        <stop position="1">
-          <color theme="0"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.59996337778862885"/>
@@ -218,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -304,21 +288,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -334,19 +303,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -415,7 +371,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -424,33 +380,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -466,9 +413,6 @@
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -502,50 +446,50 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="6" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -943,10 +887,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="L11" sqref="A10:L11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -963,61 +907,60 @@
     <col min="10" max="10" width="16.85546875" style="4" customWidth="1"/>
     <col min="11" max="11" width="23.7109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="21.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-    </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1031,272 +974,257 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="28" t="s">
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="B8" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="36" t="s">
+      <c r="G8" s="34"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="34" t="s">
+      <c r="G9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="7" t="s">
+      <c r="K9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" s="7" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+    </row>
+    <row r="11" spans="1:12" s="7" customFormat="1" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="41"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="40"/>
+    </row>
+    <row r="12" spans="1:12" s="11" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" s="8" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" s="13" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="41">
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="37">
         <f>SUM(L10:L11)</f>
         <v>0</v>
       </c>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="21"/>
-    </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="21"/>
-    </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="21"/>
-    </row>
-    <row r="16" spans="1:13" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="21"/>
-    </row>
-    <row r="17" spans="1:13" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="21"/>
-    </row>
-    <row r="18" spans="1:13" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="21"/>
-    </row>
-    <row r="19" spans="1:13" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L20" s="22"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L22" s="23"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L24" s="23"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L27" s="23"/>
+    </row>
+    <row r="13" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="17"/>
+    </row>
+    <row r="16" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="17"/>
+    </row>
+    <row r="17" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="17"/>
+    </row>
+    <row r="18" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="17"/>
+    </row>
+    <row r="19" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="17"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="18"/>
+    </row>
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L22" s="19"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L24" s="19"/>
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1307,9 +1235,6 @@
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.11811023622047245" bottom="0.11811023622047245" header="0.11811023622047245" footer="0.11811023622047245"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="12" max="1048575" man="1"/>
-  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EXCEL MEJORADO CTAS GRALES
</commit_message>
<xml_diff>
--- a/reportes/controladores_fpdf/template_contabilidad_1.xlsx
+++ b/reportes/controladores_fpdf/template_contabilidad_1.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">S.Gral.2018Cta.!$E$7:$E$27</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,9 +73,6 @@
     <t>ACDO.</t>
   </si>
   <si>
-    <t>TOTAL MES DE DICIEMBRE DE 2016</t>
-  </si>
-  <si>
     <t>DOCUMENTACION DE</t>
   </si>
   <si>
@@ -98,6 +95,11 @@
   </si>
   <si>
     <t>UNIDAD DE SUPERFICIE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+TOTAL MES DE DICIEMBRE DE 2016
+</t>
   </si>
 </sst>
 </file>
@@ -107,7 +109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +155,18 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Lucida Sans Unicode"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -370,11 +384,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,7 +500,19 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -527,8 +552,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>567651</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>151076</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>112591</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -575,10 +600,10 @@
       <xdr:rowOff>57728</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>165486</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1452803</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -889,61 +914,61 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="E6" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="59.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="23.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="18.85546875" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:12" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+    </row>
+    <row r="2" spans="1:12" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+    </row>
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
@@ -959,24 +984,24 @@
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
+      <c r="D4" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
-        <v>3</v>
-      </c>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>
@@ -989,248 +1014,249 @@
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22" t="s">
+    <row r="6" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="24" t="s">
+      <c r="L7" s="21"/>
+    </row>
+    <row r="8" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="B8" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="22"/>
-    </row>
-    <row r="8" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="31" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="40"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
+    </row>
+    <row r="12" spans="1:12" s="10" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="40"/>
-    </row>
-    <row r="11" spans="1:12" s="7" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="40"/>
-    </row>
-    <row r="12" spans="1:12" s="11" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="37">
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="36">
         <f>SUM(L10:L11)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="17"/>
-    </row>
-    <row r="14" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="17"/>
-    </row>
-    <row r="15" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="17"/>
-    </row>
-    <row r="16" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="17"/>
-    </row>
-    <row r="17" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="17"/>
-    </row>
-    <row r="18" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="17"/>
-    </row>
-    <row r="19" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="17"/>
-    </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L20" s="18"/>
-    </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L22" s="19"/>
-    </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L24" s="19"/>
-    </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L27" s="19"/>
+    <row r="13" spans="1:12" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="16"/>
+    </row>
+    <row r="14" spans="1:12" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="16"/>
+    </row>
+    <row r="15" spans="1:12" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="16"/>
+    </row>
+    <row r="16" spans="1:12" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="16"/>
+    </row>
+    <row r="18" spans="1:12" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19" spans="1:12" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L20" s="17"/>
+    </row>
+    <row r="22" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="L22" s="18"/>
+    </row>
+    <row r="24" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="L24" s="18"/>
+    </row>
+    <row r="27" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="L27" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A5:L5"/>
+    <mergeCell ref="D4:J4"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.11811023622047245" bottom="0.11811023622047245" header="0.11811023622047245" footer="0.11811023622047245"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>

</xml_diff>